<commit_message>
Update: Add new business trips data for 2025
</commit_message>
<xml_diff>
--- a/출장보고서2005.xlsx
+++ b/출장보고서2005.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsung\work_action\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BA3883D-5899-4879-8479-3DA184384DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBDF80E-187F-4A0C-A069-CFDEDBCB2268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1837" yWindow="1837" windowWidth="16201" windowHeight="9308" xr2:uid="{000828AA-869D-48F6-AAA4-2DAD6358D444}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{000828AA-869D-48F6-AAA4-2DAD6358D444}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
   <si>
     <t>보고서ID</t>
   </si>
@@ -241,6 +241,66 @@
   </si>
   <si>
     <t>김득중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대구시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>참외 작목현황</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김상걸, 차수호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">참외 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김상걸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>밀양</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하우스감사 시세 동향 및 출하 상담</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김용보, 이용수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김용보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전남</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해남군</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>봄동배추, 대파 줄하독려</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김언중 김기영</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배추,대파</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -608,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C59988-E790-41F3-925B-B01E4D678E24}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -1046,6 +1106,111 @@
         <v>54</v>
       </c>
     </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45693</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45693</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" s="1">
+        <v>45694</v>
+      </c>
+      <c r="K13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45693</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45693</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" s="1">
+        <v>45694</v>
+      </c>
+      <c r="K14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45693</v>
+      </c>
+      <c r="C15" s="1">
+        <v>45693</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J15" s="1">
+        <v>45694</v>
+      </c>
+      <c r="K15" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>